<commit_message>
Cambios en carpetas Models, GUI, Controllers
</commit_message>
<xml_diff>
--- a/Assets/Templates/FORMULARIOS_IQGeoSpatial.xlsx
+++ b/Assets/Templates/FORMULARIOS_IQGeoSpatial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Development\Projects\IQ GeoSpatial Technology\IQ GeoSpatial Pro V-2.2.0\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1C9F98-BCAE-48C5-9F5D-B630B4D7FBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C710F57F-CAD1-45CC-9BE3-92219B8BE517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2826F406-C9C4-4B7C-BFB3-29364BC2B672}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2826F406-C9C4-4B7C-BFB3-29364BC2B672}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMULARIO 001" sheetId="1" r:id="rId1"/>
@@ -1063,7 +1063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1098,36 +1098,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,12 +1140,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2014,196 +2013,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="18">
         <v>76543210</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="18">
         <v>987654321</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="34"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="18">
         <v>1000701</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="18">
         <v>1000702</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="18">
         <v>1000703</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="18"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="18"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="18"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="18"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2240,22 +2239,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="33" t="str">
+      <c r="B2" s="23" t="str">
         <f>'FORMULARIO 001'!B2</f>
         <v>IQ GeoSpatial Technology</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14">
@@ -2264,7 +2263,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="14" t="str">
@@ -2273,7 +2272,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -2281,7 +2280,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -2289,7 +2288,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -2297,145 +2296,145 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="24" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="str">
+      <c r="A10" s="22" t="str">
         <f>IF('FORMULARIO 001'!A18&lt;&gt;"",'FORMULARIO 001'!A18,"")</f>
         <v>PUNTO_1</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="25">
         <f>IF('FORMULARIO 001'!B18&gt;=1,'FORMULARIO 001'!B18,"")</f>
         <v>1000701</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="str">
+      <c r="A11" s="22" t="str">
         <f>IF('FORMULARIO 001'!A19&lt;&gt;"",'FORMULARIO 001'!A19,"")</f>
         <v>PUNTO_2</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="25">
         <f>IF('FORMULARIO 001'!B19&gt;=1,'FORMULARIO 001'!B19,"")</f>
         <v>1000702</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="str">
+      <c r="A12" s="22" t="str">
         <f>IF('FORMULARIO 001'!A20&lt;&gt;"",'FORMULARIO 001'!A20,"")</f>
         <v>PUNTO_3</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="25">
         <f>IF('FORMULARIO 001'!B20&gt;=1,'FORMULARIO 001'!B20,"")</f>
         <v>1000703</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="str">
+      <c r="A13" s="22" t="str">
         <f>IF('FORMULARIO 001'!A21&lt;&gt;"",'FORMULARIO 001'!A21,"")</f>
         <v/>
       </c>
-      <c r="B13" s="35" t="str">
+      <c r="B13" s="25" t="str">
         <f>IF('FORMULARIO 001'!B21&gt;=1,'FORMULARIO 001'!B21,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="str">
+      <c r="A14" s="22" t="str">
         <f>IF('FORMULARIO 001'!A22&lt;&gt;"",'FORMULARIO 001'!A22,"")</f>
         <v/>
       </c>
-      <c r="B14" s="35" t="str">
+      <c r="B14" s="25" t="str">
         <f>IF('FORMULARIO 001'!B22&gt;=1,'FORMULARIO 001'!B22,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="str">
+      <c r="A15" s="22" t="str">
         <f>IF('FORMULARIO 001'!A23&lt;&gt;"",'FORMULARIO 001'!A23,"")</f>
         <v/>
       </c>
-      <c r="B15" s="35" t="str">
+      <c r="B15" s="25" t="str">
         <f>IF('FORMULARIO 001'!B23&gt;=1,'FORMULARIO 001'!B23,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="str">
+      <c r="A16" s="16" t="str">
         <f>IF('FORMULARIO 001'!A24&lt;&gt;"",'FORMULARIO 001'!A24,"")</f>
         <v/>
       </c>
-      <c r="B16" s="35" t="str">
+      <c r="B16" s="25" t="str">
         <f>IF('FORMULARIO 001'!B24&gt;=1,'FORMULARIO 001'!B24,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="str">
+      <c r="A17" s="16" t="str">
         <f>IF('FORMULARIO 001'!A25&lt;&gt;"",'FORMULARIO 001'!A25,"")</f>
         <v/>
       </c>
-      <c r="B17" s="35" t="str">
+      <c r="B17" s="25" t="str">
         <f>IF('FORMULARIO 001'!B25&gt;=1,'FORMULARIO 001'!B25,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="str">
+      <c r="A18" s="16" t="str">
         <f>IF('FORMULARIO 001'!A26&lt;&gt;"",'FORMULARIO 001'!A26,"")</f>
         <v/>
       </c>
-      <c r="B18" s="35" t="str">
+      <c r="B18" s="25" t="str">
         <f>IF('FORMULARIO 001'!B26&gt;=1,'FORMULARIO 001'!B26,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="str">
+      <c r="A19" s="16" t="str">
         <f>IF('FORMULARIO 001'!A27&lt;&gt;"",'FORMULARIO 001'!A27,"")</f>
         <v/>
       </c>
-      <c r="B19" s="35" t="str">
+      <c r="B19" s="25" t="str">
         <f>IF('FORMULARIO 001'!B27&gt;=1,'FORMULARIO 001'!B27,"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="str">
+      <c r="A20" s="16" t="str">
         <f>IF('FORMULARIO 001'!A28&lt;&gt;"",'FORMULARIO 001'!A28,"")</f>
         <v/>
       </c>
-      <c r="B20" s="35" t="str">
+      <c r="B20" s="25" t="str">
         <f>IF('FORMULARIO 001'!B28&gt;=1,'FORMULARIO 001'!B28,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="16" t="str">
         <f>IF('FORMULARIO 001'!A29&lt;&gt;"",'FORMULARIO 001'!A29,"")</f>
         <v/>
       </c>
-      <c r="B21" s="35" t="str">
+      <c r="B21" s="25" t="str">
         <f>IF('FORMULARIO 001'!B29&gt;=1,'FORMULARIO 001'!B29,"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="str">
+      <c r="A22" s="16" t="str">
         <f>IF('FORMULARIO 001'!A30&lt;&gt;"",'FORMULARIO 001'!A30,"")</f>
         <v/>
       </c>
-      <c r="B22" s="35" t="str">
+      <c r="B22" s="25" t="str">
         <f>IF('FORMULARIO 001'!B30&gt;=1,'FORMULARIO 001'!B30,"")</f>
         <v/>
       </c>
@@ -2458,8 +2457,8 @@
   </sheetPr>
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,28 +2474,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:20" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -2506,18 +2505,18 @@
       <c r="N2" s="15"/>
     </row>
     <row r="3" spans="1:20" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="43" t="str">
+      <c r="B3" s="32" t="str">
         <f>'FORMULARIO 001'!B2</f>
         <v>IQ GeoSpatial Technology</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -2527,18 +2526,18 @@
       <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:20" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>'FORMULARIO 001'!B8</f>
         <v>GNSS</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2548,18 +2547,18 @@
       <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>'FORMULARIO 001'!B9</f>
         <v>MODELO_X</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -2569,18 +2568,18 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>'FORMULARIO 001'!B10</f>
         <v>SOUTH</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -2590,18 +2589,18 @@
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>'FORMULARIO 001'!B11</f>
         <v>GNSS</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -2611,18 +2610,18 @@
       <c r="N7" s="15"/>
     </row>
     <row r="8" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>'FORMULARIO 001'!B12</f>
         <v>ANT_200</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
@@ -2632,18 +2631,18 @@
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="38" t="str">
+      <c r="B9" s="28" t="str">
         <f>'FORMULARIO 001'!B13</f>
         <v>SOUTH</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
@@ -2653,7 +2652,7 @@
       <c r="N9" s="15"/>
     </row>
     <row r="10" spans="1:20" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2665,9 +2664,9 @@
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -2677,7 +2676,7 @@
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2689,9 +2688,9 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -2701,7 +2700,7 @@
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="4">
@@ -2713,9 +2712,9 @@
       <c r="D12" s="4">
         <v>1.8</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -2725,7 +2724,7 @@
       <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4">
@@ -2737,9 +2736,9 @@
       <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -2749,7 +2748,7 @@
       <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:20" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2761,9 +2760,9 @@
       <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -2773,7 +2772,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="6">
@@ -2834,7 +2833,7 @@
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -2864,7 +2863,7 @@
       <c r="T16" s="5"/>
     </row>
     <row r="17" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -2889,7 +2888,7 @@
       <c r="O17" s="7"/>
     </row>
     <row r="18" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -2914,7 +2913,7 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="6">
@@ -2939,7 +2938,7 @@
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="6">
@@ -2964,7 +2963,7 @@
       <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="11">
@@ -2989,7 +2988,7 @@
       <c r="O21" s="7"/>
     </row>
     <row r="22" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="11">
@@ -3014,7 +3013,7 @@
       <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="6">
@@ -3039,38 +3038,38 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" spans="1:15" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
     </row>
     <row r="25" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -3104,7 +3103,7 @@
   </sheetPr>
   <dimension ref="D1:T26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -3112,239 +3111,239 @@
   <sheetData>
     <row r="1" spans="4:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="3" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
     </row>
     <row r="4" spans="4:20" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
     </row>
     <row r="5" spans="4:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
     </row>
     <row r="8" spans="4:20" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="20" t="s">
+      <c r="N9" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
     </row>
     <row r="10" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
     </row>
     <row r="11" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
     </row>
     <row r="12" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
     </row>
     <row r="13" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
     </row>
     <row r="14" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
     </row>
     <row r="15" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
     </row>
     <row r="25" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="J25" s="22" t="s">
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="J25" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="P25" s="23" t="s">
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="P25" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
     </row>
     <row r="26" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>